<commit_message>
EntityFinder Visitor -> build query to find owner of an imported entity
</commit_message>
<xml_diff>
--- a/Composantes.xlsx
+++ b/Composantes.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\new_age\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="9075"/>
   </bookViews>
   <sheets>
-    <sheet name="Détails Composantes" sheetId="1" r:id="rId4"/>
+    <sheet name="Détails Composantes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="26">
   <si>
     <t>Composantes</t>
   </si>
@@ -98,14 +102,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -116,14 +115,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -137,24 +139,30 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -444,90 +452,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283447000000001" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9.283447000000001" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283447000000001" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="29.421387" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="9.283447000000001" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="9.283447000000001" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -539,26 +542,26 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -582,20 +585,20 @@
       <c r="K4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -632,7 +635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -645,7 +648,6 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6"/>
       <c r="F6">
         <v>2</v>
       </c>
@@ -685,9 +687,8 @@
       <c r="R6">
         <v>20</v>
       </c>
-      <c r="S6"/>
-    </row>
-    <row r="7" spans="1:19">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -700,7 +701,6 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7"/>
       <c r="F7">
         <v>2</v>
       </c>
@@ -740,9 +740,8 @@
       <c r="R7">
         <v>25</v>
       </c>
-      <c r="S7"/>
-    </row>
-    <row r="8" spans="1:19">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -755,7 +754,6 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8"/>
       <c r="F8">
         <v>2</v>
       </c>
@@ -795,9 +793,8 @@
       <c r="R8">
         <v>15</v>
       </c>
-      <c r="S8"/>
-    </row>
-    <row r="9" spans="1:19">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -810,7 +807,6 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9"/>
       <c r="F9">
         <v>2</v>
       </c>
@@ -850,9 +846,8 @@
       <c r="R9">
         <v>15</v>
       </c>
-      <c r="S9"/>
-    </row>
-    <row r="10" spans="1:19">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -865,7 +860,6 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10"/>
       <c r="F10">
         <v>2</v>
       </c>
@@ -905,9 +899,8 @@
       <c r="R10">
         <v>20</v>
       </c>
-      <c r="S10"/>
-    </row>
-    <row r="11" spans="1:19">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -920,7 +913,6 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11"/>
       <c r="F11">
         <v>2</v>
       </c>
@@ -960,9 +952,8 @@
       <c r="R11">
         <v>20</v>
       </c>
-      <c r="S11"/>
-    </row>
-    <row r="12" spans="1:19">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -975,7 +966,6 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12"/>
       <c r="F12">
         <v>2</v>
       </c>
@@ -1015,9 +1005,8 @@
       <c r="R12">
         <v>8</v>
       </c>
-      <c r="S12"/>
-    </row>
-    <row r="13" spans="1:19">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1030,7 +1019,6 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13"/>
       <c r="F13">
         <v>2</v>
       </c>
@@ -1070,9 +1058,8 @@
       <c r="R13">
         <v>22</v>
       </c>
-      <c r="S13"/>
-    </row>
-    <row r="14" spans="1:19">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1085,7 +1072,6 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14"/>
       <c r="F14">
         <v>2</v>
       </c>
@@ -1125,9 +1111,8 @@
       <c r="R14">
         <v>22</v>
       </c>
-      <c r="S14"/>
-    </row>
-    <row r="15" spans="1:19">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1140,7 +1125,6 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15"/>
       <c r="F15">
         <v>2</v>
       </c>
@@ -1180,9 +1164,8 @@
       <c r="R15">
         <v>12</v>
       </c>
-      <c r="S15"/>
-    </row>
-    <row r="16" spans="1:19">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1195,7 +1178,6 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16"/>
       <c r="F16">
         <v>2</v>
       </c>
@@ -1235,9 +1217,8 @@
       <c r="R16">
         <v>18</v>
       </c>
-      <c r="S16"/>
-    </row>
-    <row r="17" spans="1:19">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1250,7 +1231,6 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17"/>
       <c r="F17">
         <v>2</v>
       </c>
@@ -1290,9 +1270,8 @@
       <c r="R17">
         <v>22</v>
       </c>
-      <c r="S17"/>
-    </row>
-    <row r="18" spans="1:19">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1305,7 +1284,6 @@
       <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="E18"/>
       <c r="F18">
         <v>2</v>
       </c>
@@ -1334,7 +1312,7 @@
         <v>16</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>1500</v>
       </c>
       <c r="P18" t="s">
         <v>19</v>
@@ -1345,9 +1323,8 @@
       <c r="R18">
         <v>20</v>
       </c>
-      <c r="S18"/>
-    </row>
-    <row r="19" spans="1:19">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1360,7 +1337,6 @@
       <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="E19"/>
       <c r="F19">
         <v>2</v>
       </c>
@@ -1400,9 +1376,8 @@
       <c r="R19">
         <v>25</v>
       </c>
-      <c r="S19"/>
-    </row>
-    <row r="20" spans="1:19">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1415,7 +1390,6 @@
       <c r="D20" t="s">
         <v>25</v>
       </c>
-      <c r="E20"/>
       <c r="F20">
         <v>2</v>
       </c>
@@ -1455,9 +1429,8 @@
       <c r="R20">
         <v>15</v>
       </c>
-      <c r="S20"/>
-    </row>
-    <row r="21" spans="1:19">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1470,7 +1443,6 @@
       <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E21"/>
       <c r="F21">
         <v>2</v>
       </c>
@@ -1510,9 +1482,8 @@
       <c r="R21">
         <v>15</v>
       </c>
-      <c r="S21"/>
-    </row>
-    <row r="22" spans="1:19">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1525,7 +1496,6 @@
       <c r="D22" t="s">
         <v>25</v>
       </c>
-      <c r="E22"/>
       <c r="F22">
         <v>2</v>
       </c>
@@ -1565,9 +1535,8 @@
       <c r="R22">
         <v>20</v>
       </c>
-      <c r="S22"/>
-    </row>
-    <row r="23" spans="1:19">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1580,7 +1549,6 @@
       <c r="D23" t="s">
         <v>25</v>
       </c>
-      <c r="E23"/>
       <c r="F23">
         <v>2</v>
       </c>
@@ -1620,9 +1588,8 @@
       <c r="R23">
         <v>20</v>
       </c>
-      <c r="S23"/>
-    </row>
-    <row r="24" spans="1:19">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1635,7 +1602,6 @@
       <c r="D24" t="s">
         <v>25</v>
       </c>
-      <c r="E24"/>
       <c r="F24">
         <v>2</v>
       </c>
@@ -1675,9 +1641,8 @@
       <c r="R24">
         <v>8</v>
       </c>
-      <c r="S24"/>
-    </row>
-    <row r="25" spans="1:19">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1690,7 +1655,6 @@
       <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="E25"/>
       <c r="F25">
         <v>2</v>
       </c>
@@ -1730,9 +1694,8 @@
       <c r="R25">
         <v>22</v>
       </c>
-      <c r="S25"/>
-    </row>
-    <row r="26" spans="1:19">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1745,7 +1708,6 @@
       <c r="D26" t="s">
         <v>25</v>
       </c>
-      <c r="E26"/>
       <c r="F26">
         <v>2</v>
       </c>
@@ -1785,9 +1747,8 @@
       <c r="R26">
         <v>22</v>
       </c>
-      <c r="S26"/>
-    </row>
-    <row r="27" spans="1:19">
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1800,7 +1761,6 @@
       <c r="D27" t="s">
         <v>25</v>
       </c>
-      <c r="E27"/>
       <c r="F27">
         <v>2</v>
       </c>
@@ -1840,9 +1800,8 @@
       <c r="R27">
         <v>12</v>
       </c>
-      <c r="S27"/>
-    </row>
-    <row r="28" spans="1:19">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1855,7 +1814,6 @@
       <c r="D28" t="s">
         <v>25</v>
       </c>
-      <c r="E28"/>
       <c r="F28">
         <v>2</v>
       </c>
@@ -1895,9 +1853,8 @@
       <c r="R28">
         <v>18</v>
       </c>
-      <c r="S28"/>
-    </row>
-    <row r="29" spans="1:19">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1910,7 +1867,6 @@
       <c r="D29" t="s">
         <v>25</v>
       </c>
-      <c r="E29"/>
       <c r="F29">
         <v>2</v>
       </c>
@@ -1950,11 +1906,10 @@
       <c r="R29">
         <v>22</v>
       </c>
-      <c r="S29"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="6">
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="C2:S2"/>
     <mergeCell ref="F3:H3"/>
@@ -1962,16 +1917,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:S4"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>